<commit_message>
Merge the two dataframes
</commit_message>
<xml_diff>
--- a/prefinance.xlsx
+++ b/prefinance.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfaraday01\Documents\Code\fifo_aging_analysis\fifo_aging_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22B34B63-DADC-4EB0-BCC8-E5425C40B01B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D269A1-2BAA-497B-AD3A-6D97822231E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{CA992EAD-5F8B-4141-888A-13E9A85A7F21}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{CA992EAD-5F8B-4141-888A-13E9A85A7F21}"/>
   </bookViews>
   <sheets>
     <sheet name="Debits" sheetId="1" r:id="rId1"/>
@@ -36,334 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="253">
-  <si>
-    <t>Agona Amenfi</t>
-  </si>
-  <si>
-    <t>Asankragwa A</t>
-  </si>
-  <si>
-    <t>Samreboi A</t>
-  </si>
-  <si>
-    <t>Samreboi C</t>
-  </si>
-  <si>
-    <t>Samreboi D</t>
-  </si>
-  <si>
-    <t>Dunkwa A</t>
-  </si>
-  <si>
-    <t>Dunkwa B</t>
-  </si>
-  <si>
-    <t>Wassa Akropong A</t>
-  </si>
-  <si>
-    <t>Wassa Akropong B</t>
-  </si>
-  <si>
-    <t>Asankragwa B - UCGL</t>
-  </si>
-  <si>
-    <t>Manso Amanfi B - UCGL</t>
-  </si>
-  <si>
-    <t>Samreboi B -UCGL</t>
-  </si>
-  <si>
-    <t>Bepoh - UCGL</t>
-  </si>
-  <si>
-    <t>Bogoso B -UCGL</t>
-  </si>
-  <si>
-    <t>Bogoso - UCGL</t>
-  </si>
-  <si>
-    <t>Dunkwa - UCGL</t>
-  </si>
-  <si>
-    <t>Asankragwa - UCGL</t>
-  </si>
-  <si>
-    <t>Manso Amenfi A - UCGL</t>
-  </si>
-  <si>
-    <t>Samreboi - UCGL</t>
-  </si>
-  <si>
-    <t>Wassa Akropong - UCGL</t>
-  </si>
-  <si>
-    <t>Tarkwa A</t>
-  </si>
-  <si>
-    <t>Tarkwa B</t>
-  </si>
-  <si>
-    <t>Enchi B</t>
-  </si>
-  <si>
-    <t>Enchi D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dadieso </t>
-  </si>
-  <si>
-    <t>Juaboso B</t>
-  </si>
-  <si>
-    <t>Juaboso C</t>
-  </si>
-  <si>
-    <t>Juaboso D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akontombra A </t>
-  </si>
-  <si>
-    <t>Enchi A - UCGL</t>
-  </si>
-  <si>
-    <t>Enchi B - UCGL</t>
-  </si>
-  <si>
-    <t>Juaboso A - UCGL</t>
-  </si>
-  <si>
-    <t>Akontombra B - UCGL</t>
-  </si>
-  <si>
-    <t>Juaboso C - UCGL</t>
-  </si>
-  <si>
-    <t>Sefwi Asafo</t>
-  </si>
-  <si>
-    <t>Asawinso A</t>
-  </si>
-  <si>
-    <t>Asawinso B</t>
-  </si>
-  <si>
-    <t>Asawinso C</t>
-  </si>
-  <si>
-    <t>Boako A</t>
-  </si>
-  <si>
-    <t>Boako B</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sefwi Wiawso </t>
-  </si>
-  <si>
-    <t>Adabokrom</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Debiso </t>
-  </si>
-  <si>
-    <t>Elluokrom B</t>
-  </si>
-  <si>
-    <t>Essam</t>
-  </si>
-  <si>
-    <t>Sefwi Bekwai</t>
-  </si>
-  <si>
-    <t>Bonsu B</t>
-  </si>
-  <si>
-    <t>Proso A</t>
-  </si>
-  <si>
-    <t>Proso B</t>
-  </si>
-  <si>
-    <t>Asempanaye - UCGL</t>
-  </si>
-  <si>
-    <t>Elluokrom A -UCGL</t>
-  </si>
-  <si>
-    <t>Bonsu A - UCGL</t>
-  </si>
-  <si>
-    <t>Bonsu B - UCGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bibiani </t>
-  </si>
-  <si>
-    <t>Diaso C</t>
-  </si>
-  <si>
-    <t>Sankore A</t>
-  </si>
-  <si>
-    <t>Sankore B</t>
-  </si>
-  <si>
-    <t>Kukuom</t>
-  </si>
-  <si>
-    <t>Asumura A</t>
-  </si>
-  <si>
-    <t>Asumura B</t>
-  </si>
-  <si>
-    <t>Asumura C</t>
-  </si>
-  <si>
-    <t>Kasapin B</t>
-  </si>
-  <si>
-    <t>Goaso B</t>
-  </si>
-  <si>
-    <t>Asumura - UCGL</t>
-  </si>
-  <si>
-    <t>Goaso A - UCGL</t>
-  </si>
-  <si>
-    <t>Diaso - UCGL</t>
-  </si>
-  <si>
-    <t>Kasapin - UCGL</t>
-  </si>
-  <si>
-    <t>Goaso B -UCGL</t>
-  </si>
-  <si>
-    <t>Sunyani -UCGL</t>
-  </si>
-  <si>
-    <t>Tepa A</t>
-  </si>
-  <si>
-    <t>Antoakrom A</t>
-  </si>
-  <si>
-    <t>Antoakrom B</t>
-  </si>
-  <si>
-    <t>Antoakrom C</t>
-  </si>
-  <si>
-    <t>Mankranso</t>
-  </si>
-  <si>
-    <t>Konongo</t>
-  </si>
-  <si>
-    <t>Nkawie</t>
-  </si>
-  <si>
-    <t>Offinso - UCGL</t>
-  </si>
-  <si>
-    <t>Abenase - UCGL</t>
-  </si>
-  <si>
-    <t>Antoakrom  - UCGL</t>
-  </si>
-  <si>
-    <t>Tepa B -UCGL</t>
-  </si>
-  <si>
-    <t>Juaso - UCGL</t>
-  </si>
-  <si>
-    <t>Ashanti Agona - UCGL</t>
-  </si>
-  <si>
-    <t>Effiduase - UCGL</t>
-  </si>
-  <si>
-    <t>Nyinahin - UCGL</t>
-  </si>
-  <si>
-    <t>Ofoase - UCGL</t>
-  </si>
-  <si>
-    <t>Papase - UCGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Asante Bekwai </t>
-  </si>
-  <si>
-    <t>New Edubiase A</t>
-  </si>
-  <si>
-    <t>New Edubiase B</t>
-  </si>
-  <si>
-    <t>Twifo Praso</t>
-  </si>
-  <si>
-    <t>Assin Fosu</t>
-  </si>
-  <si>
-    <t>Ateiku</t>
-  </si>
-  <si>
-    <t>Breman Asikuma - UCGL</t>
-  </si>
-  <si>
-    <t>Brakwa - UCGL</t>
-  </si>
-  <si>
-    <t>Obuasi B - UCGL</t>
-  </si>
-  <si>
-    <t>Assin Breku - UCGL</t>
-  </si>
-  <si>
-    <t>Twifo Nyinase - UCGL</t>
-  </si>
-  <si>
-    <t>Obuasi - UCGL</t>
-  </si>
-  <si>
-    <t>New Edubiase A - UCGL</t>
-  </si>
-  <si>
-    <t>New Edubiase B - UCGL</t>
-  </si>
-  <si>
-    <t>Assin Fosu B - UCGL</t>
-  </si>
-  <si>
-    <t>Twifo Praso - UCGL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Akim Oda </t>
-  </si>
-  <si>
-    <t>Asamankese</t>
-  </si>
-  <si>
-    <t>Kade A</t>
-  </si>
-  <si>
-    <t>Suhum B</t>
-  </si>
-  <si>
-    <t>Nkawkaw - UCGL</t>
-  </si>
-  <si>
-    <t>Suhum - UCGL</t>
-  </si>
-  <si>
-    <t>Kyebi - UCGL</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="143">
   <si>
     <t>1-Oct-21</t>
   </si>
@@ -459,9 +132,6 @@
   </si>
   <si>
     <t>6-May-22</t>
-  </si>
-  <si>
-    <t>District</t>
   </si>
   <si>
     <t>Total Credit</t>
@@ -1148,8 +818,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A41A6FD-3748-43BF-9423-759042313133}">
   <dimension ref="A1:AG110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection sqref="A1:A110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1159,108 +829,108 @@
   <sheetData>
     <row r="1" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>109</v>
+        <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>110</v>
+        <v>1</v>
       </c>
       <c r="D1" t="s">
-        <v>111</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
-        <v>112</v>
+        <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>113</v>
+        <v>4</v>
       </c>
       <c r="G1" t="s">
-        <v>114</v>
+        <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>6</v>
       </c>
       <c r="I1" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="J1" t="s">
-        <v>117</v>
+        <v>8</v>
       </c>
       <c r="K1" t="s">
-        <v>118</v>
+        <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>119</v>
+        <v>10</v>
       </c>
       <c r="M1" t="s">
-        <v>120</v>
+        <v>11</v>
       </c>
       <c r="N1" t="s">
-        <v>121</v>
+        <v>12</v>
       </c>
       <c r="O1" t="s">
-        <v>122</v>
+        <v>13</v>
       </c>
       <c r="P1" t="s">
-        <v>123</v>
+        <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>124</v>
+        <v>15</v>
       </c>
       <c r="R1" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="S1" t="s">
-        <v>126</v>
+        <v>17</v>
       </c>
       <c r="T1" t="s">
-        <v>127</v>
+        <v>18</v>
       </c>
       <c r="U1" t="s">
-        <v>128</v>
+        <v>19</v>
       </c>
       <c r="V1" t="s">
-        <v>129</v>
+        <v>20</v>
       </c>
       <c r="W1" t="s">
-        <v>130</v>
+        <v>21</v>
       </c>
       <c r="X1" t="s">
-        <v>131</v>
+        <v>22</v>
       </c>
       <c r="Y1" t="s">
-        <v>132</v>
+        <v>23</v>
       </c>
       <c r="Z1" t="s">
-        <v>133</v>
+        <v>24</v>
       </c>
       <c r="AA1" t="s">
-        <v>134</v>
+        <v>25</v>
       </c>
       <c r="AB1" t="s">
-        <v>135</v>
+        <v>26</v>
       </c>
       <c r="AC1" t="s">
-        <v>136</v>
+        <v>27</v>
       </c>
       <c r="AD1" t="s">
-        <v>137</v>
+        <v>28</v>
       </c>
       <c r="AE1" t="s">
-        <v>138</v>
+        <v>29</v>
       </c>
       <c r="AF1" t="s">
-        <v>139</v>
+        <v>30</v>
       </c>
       <c r="AG1" t="s">
-        <v>140</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>50</v>
@@ -1361,7 +1031,7 @@
     </row>
     <row r="3" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>200</v>
@@ -1462,7 +1132,7 @@
     </row>
     <row r="4" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>400</v>
@@ -1563,7 +1233,7 @@
     </row>
     <row r="5" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>147</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>600</v>
@@ -1664,7 +1334,7 @@
     </row>
     <row r="6" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>148</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1765,7 +1435,7 @@
     </row>
     <row r="7" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>149</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>500</v>
@@ -1866,7 +1536,7 @@
     </row>
     <row r="8" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>150</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>65</v>
@@ -1967,7 +1637,7 @@
     </row>
     <row r="9" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>151</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>300</v>
@@ -2068,7 +1738,7 @@
     </row>
     <row r="10" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>152</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -2169,7 +1839,7 @@
     </row>
     <row r="11" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>153</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>400</v>
@@ -2270,7 +1940,7 @@
     </row>
     <row r="12" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>154</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -2371,7 +2041,7 @@
     </row>
     <row r="13" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>155</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -2472,7 +2142,7 @@
     </row>
     <row r="14" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>156</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>300</v>
@@ -2573,7 +2243,7 @@
     </row>
     <row r="15" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>157</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>300</v>
@@ -2674,7 +2344,7 @@
     </row>
     <row r="16" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>158</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -2775,7 +2445,7 @@
     </row>
     <row r="17" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>159</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>300</v>
@@ -2876,7 +2546,7 @@
     </row>
     <row r="18" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>160</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>300</v>
@@ -2977,7 +2647,7 @@
     </row>
     <row r="19" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>161</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>0</v>
@@ -3078,7 +2748,7 @@
     </row>
     <row r="20" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>162</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -3179,7 +2849,7 @@
     </row>
     <row r="21" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>163</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>400</v>
@@ -3280,7 +2950,7 @@
     </row>
     <row r="22" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>164</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>400</v>
@@ -3381,7 +3051,7 @@
     </row>
     <row r="23" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>800</v>
@@ -3482,7 +3152,7 @@
     </row>
     <row r="24" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>166</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>800</v>
@@ -3583,7 +3253,7 @@
     </row>
     <row r="25" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>167</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>300</v>
@@ -3684,7 +3354,7 @@
     </row>
     <row r="26" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>168</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>400</v>
@@ -3785,7 +3455,7 @@
     </row>
     <row r="27" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>169</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -3886,7 +3556,7 @@
     </row>
     <row r="28" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>170</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>100</v>
@@ -3987,7 +3657,7 @@
     </row>
     <row r="29" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>171</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>0</v>
@@ -4088,7 +3758,7 @@
     </row>
     <row r="30" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>172</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>300</v>
@@ -4189,7 +3859,7 @@
     </row>
     <row r="31" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>173</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>400</v>
@@ -4290,7 +3960,7 @@
     </row>
     <row r="32" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>174</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>400</v>
@@ -4391,7 +4061,7 @@
     </row>
     <row r="33" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>175</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>0</v>
@@ -4492,7 +4162,7 @@
     </row>
     <row r="34" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>176</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4593,7 +4263,7 @@
     </row>
     <row r="35" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>177</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>100</v>
@@ -4694,7 +4364,7 @@
     </row>
     <row r="36" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>178</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>50</v>
@@ -4795,7 +4465,7 @@
     </row>
     <row r="37" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>179</v>
+        <v>69</v>
       </c>
       <c r="B37">
         <v>250</v>
@@ -4896,7 +4566,7 @@
     </row>
     <row r="38" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>180</v>
+        <v>70</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4997,7 +4667,7 @@
     </row>
     <row r="39" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>181</v>
+        <v>71</v>
       </c>
       <c r="B39">
         <v>50</v>
@@ -5098,7 +4768,7 @@
     </row>
     <row r="40" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>182</v>
+        <v>72</v>
       </c>
       <c r="B40">
         <v>42</v>
@@ -5199,7 +4869,7 @@
     </row>
     <row r="41" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>183</v>
+        <v>73</v>
       </c>
       <c r="B41">
         <v>150</v>
@@ -5300,7 +4970,7 @@
     </row>
     <row r="42" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>184</v>
+        <v>74</v>
       </c>
       <c r="B42">
         <v>54</v>
@@ -5401,7 +5071,7 @@
     </row>
     <row r="43" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>185</v>
+        <v>75</v>
       </c>
       <c r="B43">
         <v>199</v>
@@ -5502,7 +5172,7 @@
     </row>
     <row r="44" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>186</v>
+        <v>76</v>
       </c>
       <c r="B44">
         <v>200</v>
@@ -5603,7 +5273,7 @@
     </row>
     <row r="45" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>187</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>200</v>
@@ -5704,7 +5374,7 @@
     </row>
     <row r="46" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>188</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>200</v>
@@ -5805,7 +5475,7 @@
     </row>
     <row r="47" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>189</v>
+        <v>79</v>
       </c>
       <c r="B47">
         <v>36</v>
@@ -5906,7 +5576,7 @@
     </row>
     <row r="48" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>190</v>
+        <v>80</v>
       </c>
       <c r="B48">
         <v>299</v>
@@ -6007,7 +5677,7 @@
     </row>
     <row r="49" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>191</v>
+        <v>81</v>
       </c>
       <c r="B49">
         <v>130</v>
@@ -6108,7 +5778,7 @@
     </row>
     <row r="50" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>192</v>
+        <v>82</v>
       </c>
       <c r="B50">
         <v>100</v>
@@ -6209,7 +5879,7 @@
     </row>
     <row r="51" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>193</v>
+        <v>83</v>
       </c>
       <c r="B51">
         <v>0</v>
@@ -6310,7 +5980,7 @@
     </row>
     <row r="52" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>194</v>
+        <v>84</v>
       </c>
       <c r="B52">
         <v>0</v>
@@ -6411,7 +6081,7 @@
     </row>
     <row r="53" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>195</v>
+        <v>85</v>
       </c>
       <c r="B53">
         <v>0</v>
@@ -6512,7 +6182,7 @@
     </row>
     <row r="54" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>196</v>
+        <v>86</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -6613,7 +6283,7 @@
     </row>
     <row r="55" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>197</v>
+        <v>87</v>
       </c>
       <c r="B55">
         <v>200</v>
@@ -6714,7 +6384,7 @@
     </row>
     <row r="56" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>198</v>
+        <v>88</v>
       </c>
       <c r="B56">
         <v>200</v>
@@ -6815,7 +6485,7 @@
     </row>
     <row r="57" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>199</v>
+        <v>89</v>
       </c>
       <c r="B57">
         <v>200</v>
@@ -6916,7 +6586,7 @@
     </row>
     <row r="58" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>200</v>
+        <v>90</v>
       </c>
       <c r="B58">
         <v>200</v>
@@ -7017,7 +6687,7 @@
     </row>
     <row r="59" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>201</v>
+        <v>91</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -7118,7 +6788,7 @@
     </row>
     <row r="60" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>202</v>
+        <v>92</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -7219,7 +6889,7 @@
     </row>
     <row r="61" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>203</v>
+        <v>93</v>
       </c>
       <c r="B61">
         <v>200</v>
@@ -7320,7 +6990,7 @@
     </row>
     <row r="62" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>204</v>
+        <v>94</v>
       </c>
       <c r="B62">
         <v>500</v>
@@ -7421,7 +7091,7 @@
     </row>
     <row r="63" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>205</v>
+        <v>95</v>
       </c>
       <c r="B63">
         <v>0</v>
@@ -7522,7 +7192,7 @@
     </row>
     <row r="64" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>206</v>
+        <v>96</v>
       </c>
       <c r="B64">
         <v>0</v>
@@ -7623,7 +7293,7 @@
     </row>
     <row r="65" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>207</v>
+        <v>97</v>
       </c>
       <c r="B65">
         <v>200</v>
@@ -7724,7 +7394,7 @@
     </row>
     <row r="66" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>208</v>
+        <v>98</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -7825,7 +7495,7 @@
     </row>
     <row r="67" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>209</v>
+        <v>99</v>
       </c>
       <c r="B67">
         <v>0</v>
@@ -7926,7 +7596,7 @@
     </row>
     <row r="68" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>210</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -8027,7 +7697,7 @@
     </row>
     <row r="69" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>211</v>
+        <v>101</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -8128,7 +7798,7 @@
     </row>
     <row r="70" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>212</v>
+        <v>102</v>
       </c>
       <c r="B70">
         <v>200</v>
@@ -8229,7 +7899,7 @@
     </row>
     <row r="71" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>213</v>
+        <v>103</v>
       </c>
       <c r="B71">
         <v>99</v>
@@ -8330,7 +8000,7 @@
     </row>
     <row r="72" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>214</v>
+        <v>104</v>
       </c>
       <c r="B72">
         <v>250</v>
@@ -8431,7 +8101,7 @@
     </row>
     <row r="73" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>215</v>
+        <v>105</v>
       </c>
       <c r="B73">
         <v>99</v>
@@ -8532,7 +8202,7 @@
     </row>
     <row r="74" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>216</v>
+        <v>106</v>
       </c>
       <c r="B74">
         <v>249</v>
@@ -8633,7 +8303,7 @@
     </row>
     <row r="75" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>217</v>
+        <v>107</v>
       </c>
       <c r="B75">
         <v>250</v>
@@ -8734,7 +8404,7 @@
     </row>
     <row r="76" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>218</v>
+        <v>108</v>
       </c>
       <c r="B76">
         <v>100</v>
@@ -8835,7 +8505,7 @@
     </row>
     <row r="77" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>219</v>
+        <v>109</v>
       </c>
       <c r="B77">
         <v>0</v>
@@ -8936,7 +8606,7 @@
     </row>
     <row r="78" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>220</v>
+        <v>110</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -9037,7 +8707,7 @@
     </row>
     <row r="79" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>221</v>
+        <v>111</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -9138,7 +8808,7 @@
     </row>
     <row r="80" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>222</v>
+        <v>112</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -9239,7 +8909,7 @@
     </row>
     <row r="81" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>223</v>
+        <v>113</v>
       </c>
       <c r="B81">
         <v>100</v>
@@ -9340,7 +9010,7 @@
     </row>
     <row r="82" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>224</v>
+        <v>114</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -9441,7 +9111,7 @@
     </row>
     <row r="83" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>225</v>
+        <v>115</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -9542,7 +9212,7 @@
     </row>
     <row r="84" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>226</v>
+        <v>116</v>
       </c>
       <c r="B84">
         <v>0</v>
@@ -9643,7 +9313,7 @@
     </row>
     <row r="85" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>227</v>
+        <v>117</v>
       </c>
       <c r="B85">
         <v>0</v>
@@ -9744,7 +9414,7 @@
     </row>
     <row r="86" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>228</v>
+        <v>118</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -9845,7 +9515,7 @@
     </row>
     <row r="87" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>229</v>
+        <v>119</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -9946,7 +9616,7 @@
     </row>
     <row r="88" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>230</v>
+        <v>120</v>
       </c>
       <c r="B88">
         <v>0</v>
@@ -10047,7 +9717,7 @@
     </row>
     <row r="89" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>231</v>
+        <v>121</v>
       </c>
       <c r="B89">
         <v>600</v>
@@ -10148,7 +9818,7 @@
     </row>
     <row r="90" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>232</v>
+        <v>122</v>
       </c>
       <c r="B90">
         <v>300</v>
@@ -10249,7 +9919,7 @@
     </row>
     <row r="91" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>233</v>
+        <v>123</v>
       </c>
       <c r="B91">
         <v>200</v>
@@ -10350,7 +10020,7 @@
     </row>
     <row r="92" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>234</v>
+        <v>124</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -10451,7 +10121,7 @@
     </row>
     <row r="93" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>235</v>
+        <v>125</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -10552,7 +10222,7 @@
     </row>
     <row r="94" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>236</v>
+        <v>126</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -10653,7 +10323,7 @@
     </row>
     <row r="95" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>237</v>
+        <v>127</v>
       </c>
       <c r="B95">
         <v>0</v>
@@ -10754,7 +10424,7 @@
     </row>
     <row r="96" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>238</v>
+        <v>128</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -10855,7 +10525,7 @@
     </row>
     <row r="97" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>239</v>
+        <v>129</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -10956,7 +10626,7 @@
     </row>
     <row r="98" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>240</v>
+        <v>130</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -11057,7 +10727,7 @@
     </row>
     <row r="99" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>241</v>
+        <v>131</v>
       </c>
       <c r="B99">
         <v>0</v>
@@ -11158,7 +10828,7 @@
     </row>
     <row r="100" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>242</v>
+        <v>132</v>
       </c>
       <c r="B100">
         <v>199</v>
@@ -11259,7 +10929,7 @@
     </row>
     <row r="101" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>243</v>
+        <v>133</v>
       </c>
       <c r="B101">
         <v>200</v>
@@ -11360,7 +11030,7 @@
     </row>
     <row r="102" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>244</v>
+        <v>134</v>
       </c>
       <c r="B102">
         <v>0</v>
@@ -11461,7 +11131,7 @@
     </row>
     <row r="103" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>245</v>
+        <v>135</v>
       </c>
       <c r="B103">
         <v>600</v>
@@ -11562,7 +11232,7 @@
     </row>
     <row r="104" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>246</v>
+        <v>136</v>
       </c>
       <c r="B104">
         <v>200</v>
@@ -11663,7 +11333,7 @@
     </row>
     <row r="105" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>247</v>
+        <v>137</v>
       </c>
       <c r="B105">
         <v>200</v>
@@ -11764,7 +11434,7 @@
     </row>
     <row r="106" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>248</v>
+        <v>138</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -11865,7 +11535,7 @@
     </row>
     <row r="107" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>249</v>
+        <v>139</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -11966,7 +11636,7 @@
     </row>
     <row r="108" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>250</v>
+        <v>140</v>
       </c>
       <c r="B108">
         <v>0</v>
@@ -12067,7 +11737,7 @@
     </row>
     <row r="109" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>251</v>
+        <v>141</v>
       </c>
       <c r="B109">
         <v>0</v>
@@ -12168,7 +11838,7 @@
     </row>
     <row r="110" spans="1:33" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>252</v>
+        <v>142</v>
       </c>
       <c r="B110">
         <v>0</v>
@@ -12276,8 +11946,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F029559-D218-485C-A850-ABE2CD583F18}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
+      <selection activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12288,15 +11958,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="B1" t="s">
-        <v>142</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>552</v>
@@ -12304,7 +11974,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>3276</v>
@@ -12312,7 +11982,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>4907</v>
@@ -12320,7 +11990,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="B5">
         <v>3504</v>
@@ -12328,7 +11998,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>38</v>
       </c>
       <c r="B6">
         <v>3765</v>
@@ -12336,7 +12006,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B7">
         <v>12379</v>
@@ -12344,7 +12014,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>40</v>
       </c>
       <c r="B8">
         <v>553</v>
@@ -12352,7 +12022,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B9">
         <v>4270</v>
@@ -12360,7 +12030,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>42</v>
       </c>
       <c r="B10">
         <v>4550</v>
@@ -12368,7 +12038,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="B11">
         <v>15519</v>
@@ -12376,7 +12046,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>44</v>
       </c>
       <c r="B12">
         <v>4915</v>
@@ -12384,7 +12054,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>45</v>
       </c>
       <c r="B13">
         <v>7834</v>
@@ -12392,7 +12062,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>46</v>
       </c>
       <c r="B14">
         <v>5687</v>
@@ -12400,7 +12070,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>47</v>
       </c>
       <c r="B15">
         <v>12530</v>
@@ -12408,7 +12078,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>48</v>
       </c>
       <c r="B16">
         <v>7551</v>
@@ -12416,7 +12086,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
       <c r="B17">
         <v>11150</v>
@@ -12424,7 +12094,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>50</v>
       </c>
       <c r="B18">
         <v>6561</v>
@@ -12432,7 +12102,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>51</v>
       </c>
       <c r="B19">
         <v>3042</v>
@@ -12440,7 +12110,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>52</v>
       </c>
       <c r="B20">
         <v>721</v>
@@ -12448,7 +12118,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>53</v>
       </c>
       <c r="B21">
         <v>15307</v>
@@ -12456,7 +12126,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>54</v>
       </c>
       <c r="B22">
         <v>4760</v>
@@ -12464,7 +12134,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>55</v>
       </c>
       <c r="B23">
         <v>13546</v>
@@ -12472,7 +12142,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>56</v>
       </c>
       <c r="B24">
         <v>11345</v>
@@ -12480,7 +12150,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>57</v>
       </c>
       <c r="B25">
         <v>7508</v>
@@ -12488,7 +12158,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>58</v>
       </c>
       <c r="B26">
         <v>14527</v>
@@ -12496,7 +12166,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>59</v>
       </c>
       <c r="B27">
         <v>3929</v>
@@ -12504,7 +12174,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>60</v>
       </c>
       <c r="B28">
         <v>3403</v>
@@ -12512,7 +12182,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>61</v>
       </c>
       <c r="B29">
         <v>6280</v>
@@ -12520,7 +12190,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B30">
         <v>1685</v>
@@ -12528,7 +12198,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>63</v>
       </c>
       <c r="B31">
         <v>7928</v>
@@ -12536,7 +12206,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>64</v>
       </c>
       <c r="B32">
         <v>7405</v>
@@ -12544,7 +12214,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B33">
         <v>2543</v>
@@ -12552,7 +12222,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="B34">
         <v>2222</v>
@@ -12560,7 +12230,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>67</v>
       </c>
       <c r="B35">
         <v>2769</v>
@@ -12568,7 +12238,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="B36">
         <v>1915</v>
@@ -12576,7 +12246,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>69</v>
       </c>
       <c r="B37">
         <v>7920</v>
@@ -12584,7 +12254,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>70</v>
       </c>
       <c r="B38">
         <v>2183</v>
@@ -12592,7 +12262,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>71</v>
       </c>
       <c r="B39">
         <v>2030</v>
@@ -12600,7 +12270,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>72</v>
       </c>
       <c r="B40">
         <v>1385</v>
@@ -12608,7 +12278,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>73</v>
       </c>
       <c r="B41">
         <v>2204</v>
@@ -12616,7 +12286,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>74</v>
       </c>
       <c r="B42">
         <v>9751</v>
@@ -12624,7 +12294,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>75</v>
       </c>
       <c r="B43">
         <v>10567</v>
@@ -12632,7 +12302,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>76</v>
       </c>
       <c r="B44">
         <v>9122</v>
@@ -12640,7 +12310,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B45">
         <v>9550</v>
@@ -12648,7 +12318,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>78</v>
       </c>
       <c r="B46">
         <v>11200</v>
@@ -12656,7 +12326,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>79</v>
       </c>
       <c r="B47">
         <v>13594</v>
@@ -12664,7 +12334,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>80</v>
       </c>
       <c r="B48">
         <v>8997</v>
@@ -12672,7 +12342,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>81</v>
       </c>
       <c r="B49">
         <v>6962</v>
@@ -12680,7 +12350,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="B50">
         <v>3511</v>
@@ -12688,7 +12358,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>83</v>
       </c>
       <c r="B51">
         <v>11271</v>
@@ -12696,7 +12366,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>84</v>
       </c>
       <c r="B52">
         <v>8320</v>
@@ -12704,7 +12374,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>85</v>
       </c>
       <c r="B53">
         <v>7160</v>
@@ -12712,7 +12382,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>86</v>
       </c>
       <c r="B54">
         <v>7278</v>
@@ -12720,7 +12390,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>87</v>
       </c>
       <c r="B55">
         <v>4450</v>
@@ -12728,7 +12398,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>88</v>
       </c>
       <c r="B56">
         <v>1118</v>
@@ -12736,7 +12406,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="B57">
         <v>12320</v>
@@ -12744,7 +12414,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>90</v>
       </c>
       <c r="B58">
         <v>6241</v>
@@ -12752,7 +12422,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>91</v>
       </c>
       <c r="B59">
         <v>35800</v>
@@ -12760,7 +12430,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>92</v>
       </c>
       <c r="B60">
         <v>4050</v>
@@ -12768,7 +12438,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>93</v>
       </c>
       <c r="B61">
         <v>6263</v>
@@ -12776,7 +12446,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>94</v>
       </c>
       <c r="B62">
         <v>34490</v>
@@ -12784,7 +12454,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>95</v>
       </c>
       <c r="B63">
         <v>11466</v>
@@ -12792,7 +12462,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>96</v>
       </c>
       <c r="B64">
         <v>9931</v>
@@ -12800,7 +12470,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>97</v>
       </c>
       <c r="B65">
         <v>5366</v>
@@ -12808,7 +12478,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>98</v>
       </c>
       <c r="B66">
         <v>2995</v>
@@ -12816,7 +12486,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>99</v>
       </c>
       <c r="B67">
         <v>33660</v>
@@ -12824,7 +12494,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>100</v>
       </c>
       <c r="B68">
         <v>9415</v>
@@ -12832,7 +12502,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>101</v>
       </c>
       <c r="B69">
         <v>37650</v>
@@ -12840,7 +12510,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>102</v>
       </c>
       <c r="B70">
         <v>36488</v>
@@ -12848,7 +12518,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="B71">
         <v>17095</v>
@@ -12856,7 +12526,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>104</v>
       </c>
       <c r="B72">
         <v>25650</v>
@@ -12864,7 +12534,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>105</v>
       </c>
       <c r="B73">
         <v>9476</v>
@@ -12872,7 +12542,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
       <c r="B74">
         <v>17000</v>
@@ -12880,7 +12550,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>107</v>
       </c>
       <c r="B75">
         <v>27047</v>
@@ -12888,7 +12558,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
       <c r="B76">
         <v>3408</v>
@@ -12896,7 +12566,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="B77">
         <v>5290</v>
@@ -12904,7 +12574,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>110</v>
       </c>
       <c r="B78">
         <v>21986</v>
@@ -12912,7 +12582,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>111</v>
       </c>
       <c r="B79">
         <v>18455</v>
@@ -12920,7 +12590,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>112</v>
       </c>
       <c r="B80">
         <v>0</v>
@@ -12928,7 +12598,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="B81">
         <v>21020</v>
@@ -12936,7 +12606,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>114</v>
       </c>
       <c r="B82">
         <v>6459</v>
@@ -12944,7 +12614,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>115</v>
       </c>
       <c r="B83">
         <v>17349</v>
@@ -12952,7 +12622,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>116</v>
       </c>
       <c r="B84">
         <v>20333</v>
@@ -12960,7 +12630,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="B85">
         <v>20300</v>
@@ -12968,7 +12638,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>118</v>
       </c>
       <c r="B86">
         <v>12543</v>
@@ -12976,7 +12646,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>119</v>
       </c>
       <c r="B87">
         <v>22190</v>
@@ -12984,7 +12654,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>120</v>
       </c>
       <c r="B88">
         <v>13716</v>
@@ -12992,7 +12662,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>121</v>
       </c>
       <c r="B89">
         <v>27437</v>
@@ -13000,7 +12670,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>122</v>
       </c>
       <c r="B90">
         <v>14505</v>
@@ -13008,7 +12678,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="B91">
         <v>16360</v>
@@ -13016,7 +12686,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>124</v>
       </c>
       <c r="B92">
         <v>4200</v>
@@ -13024,7 +12694,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>125</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -13032,7 +12702,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>126</v>
       </c>
       <c r="B94">
         <v>29939</v>
@@ -13040,7 +12710,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>127</v>
       </c>
       <c r="B95">
         <v>14888</v>
@@ -13048,7 +12718,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>128</v>
       </c>
       <c r="B96">
         <v>17016</v>
@@ -13056,7 +12726,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>129</v>
       </c>
       <c r="B97">
         <v>21600</v>
@@ -13064,7 +12734,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>130</v>
       </c>
       <c r="B98">
         <v>9182</v>
@@ -13072,7 +12742,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>131</v>
       </c>
       <c r="B99">
         <v>2664</v>
@@ -13080,7 +12750,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>132</v>
       </c>
       <c r="B100">
         <v>9250</v>
@@ -13088,7 +12758,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>133</v>
       </c>
       <c r="B101">
         <v>4638</v>
@@ -13096,7 +12766,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>134</v>
       </c>
       <c r="B102">
         <v>7515</v>
@@ -13104,7 +12774,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>135</v>
       </c>
       <c r="B103">
         <v>14250</v>
@@ -13112,7 +12782,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="B104">
         <v>22563</v>
@@ -13120,7 +12790,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>137</v>
       </c>
       <c r="B105">
         <v>23502</v>
@@ -13128,7 +12798,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>138</v>
       </c>
       <c r="B106">
         <v>9330</v>
@@ -13136,7 +12806,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>139</v>
       </c>
       <c r="B107">
         <v>18360</v>
@@ -13144,7 +12814,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>140</v>
       </c>
       <c r="B108">
         <v>27342</v>
@@ -13152,7 +12822,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>141</v>
       </c>
       <c r="B109">
         <v>8621</v>
@@ -13160,7 +12830,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>142</v>
       </c>
       <c r="B110">
         <v>18956</v>

</xml_diff>

<commit_message>
Create summary table of df
</commit_message>
<xml_diff>
--- a/prefinance.xlsx
+++ b/prefinance.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfaraday01\Documents\Code\fifo_aging_analysis\fifo_aging_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D269A1-2BAA-497B-AD3A-6D97822231E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4B06AA7-780F-4F8F-A3A4-8F6C75C003DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{CA992EAD-5F8B-4141-888A-13E9A85A7F21}"/>
   </bookViews>
@@ -471,7 +471,18 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="2">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="[$-409]d\-mmm\-yy;@"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -497,13 +508,16 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma 20" xfId="1" xr:uid="{AA2F971D-BCF9-436D-AA8E-7F0F067633FF}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -816,18 +830,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A41A6FD-3748-43BF-9423-759042313133}">
-  <dimension ref="A1:AG110"/>
+  <dimension ref="A1:AL110"/>
   <sheetViews>
-    <sheetView topLeftCell="A76" workbookViewId="0">
-      <selection sqref="A1:A110"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AP27" sqref="AP27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="20.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="36" width="9.88671875" bestFit="1" customWidth="1"/>
+    <col min="37" max="38" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -927,8 +943,23 @@
       <c r="AG1" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="2" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH1" s="1">
+        <v>44694</v>
+      </c>
+      <c r="AI1" s="1">
+        <v>44701</v>
+      </c>
+      <c r="AJ1" s="1">
+        <v>44708</v>
+      </c>
+      <c r="AK1" s="1">
+        <v>44715</v>
+      </c>
+      <c r="AL1" s="1">
+        <v>44722</v>
+      </c>
+    </row>
+    <row r="2" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1028,8 +1059,23 @@
       <c r="AG2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
+      </c>
+      <c r="AK2">
+        <v>0</v>
+      </c>
+      <c r="AL2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>35</v>
       </c>
@@ -1129,8 +1175,23 @@
       <c r="AG3">
         <v>200</v>
       </c>
-    </row>
-    <row r="4" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH3">
+        <v>150</v>
+      </c>
+      <c r="AI3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>49</v>
+      </c>
+      <c r="AK3">
+        <v>0</v>
+      </c>
+      <c r="AL3">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>36</v>
       </c>
@@ -1230,8 +1291,23 @@
       <c r="AG4">
         <v>200</v>
       </c>
-    </row>
-    <row r="5" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH4">
+        <v>300</v>
+      </c>
+      <c r="AI4">
+        <v>200</v>
+      </c>
+      <c r="AJ4">
+        <v>100</v>
+      </c>
+      <c r="AK4">
+        <v>200</v>
+      </c>
+      <c r="AL4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -1331,8 +1407,23 @@
       <c r="AG5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH5">
+        <v>0</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>0</v>
+      </c>
+      <c r="AK5">
+        <v>0</v>
+      </c>
+      <c r="AL5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>38</v>
       </c>
@@ -1432,8 +1523,23 @@
       <c r="AG6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH6">
+        <v>500</v>
+      </c>
+      <c r="AI6">
+        <v>500</v>
+      </c>
+      <c r="AJ6">
+        <v>500</v>
+      </c>
+      <c r="AK6">
+        <v>0</v>
+      </c>
+      <c r="AL6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>39</v>
       </c>
@@ -1533,8 +1639,23 @@
       <c r="AG7">
         <v>400</v>
       </c>
-    </row>
-    <row r="8" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH7">
+        <v>200</v>
+      </c>
+      <c r="AI7">
+        <v>250</v>
+      </c>
+      <c r="AJ7">
+        <v>150</v>
+      </c>
+      <c r="AK7">
+        <v>0</v>
+      </c>
+      <c r="AL7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1634,8 +1755,23 @@
       <c r="AG8">
         <v>41</v>
       </c>
-    </row>
-    <row r="9" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH8">
+        <v>29</v>
+      </c>
+      <c r="AI8">
+        <v>1</v>
+      </c>
+      <c r="AJ8">
+        <v>50</v>
+      </c>
+      <c r="AK8">
+        <v>50</v>
+      </c>
+      <c r="AL8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>41</v>
       </c>
@@ -1735,8 +1871,23 @@
       <c r="AG9">
         <v>176</v>
       </c>
-    </row>
-    <row r="10" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH9">
+        <v>50</v>
+      </c>
+      <c r="AI9">
+        <v>50</v>
+      </c>
+      <c r="AJ9">
+        <v>50</v>
+      </c>
+      <c r="AK9">
+        <v>0</v>
+      </c>
+      <c r="AL9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>42</v>
       </c>
@@ -1836,8 +1987,23 @@
       <c r="AG10">
         <v>300</v>
       </c>
-    </row>
-    <row r="11" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH10">
+        <v>100</v>
+      </c>
+      <c r="AI10">
+        <v>0</v>
+      </c>
+      <c r="AJ10">
+        <v>99</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>43</v>
       </c>
@@ -1937,8 +2103,23 @@
       <c r="AG11">
         <v>200</v>
       </c>
-    </row>
-    <row r="12" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH11">
+        <v>150</v>
+      </c>
+      <c r="AI11">
+        <v>901</v>
+      </c>
+      <c r="AJ11">
+        <v>75</v>
+      </c>
+      <c r="AK11">
+        <v>74</v>
+      </c>
+      <c r="AL11">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>44</v>
       </c>
@@ -2038,8 +2219,23 @@
       <c r="AG12">
         <v>200</v>
       </c>
-    </row>
-    <row r="13" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH12">
+        <v>198</v>
+      </c>
+      <c r="AI12">
+        <v>210</v>
+      </c>
+      <c r="AJ12">
+        <v>200</v>
+      </c>
+      <c r="AK12">
+        <v>90</v>
+      </c>
+      <c r="AL12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>45</v>
       </c>
@@ -2139,8 +2335,23 @@
       <c r="AG13">
         <v>600</v>
       </c>
-    </row>
-    <row r="14" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH13">
+        <v>801</v>
+      </c>
+      <c r="AI13">
+        <v>600</v>
+      </c>
+      <c r="AJ13">
+        <v>600</v>
+      </c>
+      <c r="AK13">
+        <v>0</v>
+      </c>
+      <c r="AL13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>46</v>
       </c>
@@ -2240,8 +2451,23 @@
       <c r="AG14">
         <v>397</v>
       </c>
-    </row>
-    <row r="15" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH14">
+        <v>396</v>
+      </c>
+      <c r="AI14">
+        <v>0</v>
+      </c>
+      <c r="AJ14">
+        <v>0</v>
+      </c>
+      <c r="AK14">
+        <v>0</v>
+      </c>
+      <c r="AL14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>47</v>
       </c>
@@ -2341,8 +2567,23 @@
       <c r="AG15">
         <v>800</v>
       </c>
-    </row>
-    <row r="16" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH15">
+        <v>1000</v>
+      </c>
+      <c r="AI15">
+        <v>500</v>
+      </c>
+      <c r="AJ15">
+        <v>300</v>
+      </c>
+      <c r="AK15">
+        <v>200</v>
+      </c>
+      <c r="AL15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>48</v>
       </c>
@@ -2442,8 +2683,23 @@
       <c r="AG16">
         <v>500</v>
       </c>
-    </row>
-    <row r="17" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH16">
+        <v>399</v>
+      </c>
+      <c r="AI16">
+        <v>249</v>
+      </c>
+      <c r="AJ16">
+        <v>299</v>
+      </c>
+      <c r="AK16">
+        <v>0</v>
+      </c>
+      <c r="AL16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>49</v>
       </c>
@@ -2543,8 +2799,23 @@
       <c r="AG17">
         <v>298</v>
       </c>
-    </row>
-    <row r="18" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH17">
+        <v>190</v>
+      </c>
+      <c r="AI17">
+        <v>107</v>
+      </c>
+      <c r="AJ17">
+        <v>200</v>
+      </c>
+      <c r="AK17">
+        <v>0</v>
+      </c>
+      <c r="AL17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>50</v>
       </c>
@@ -2644,8 +2915,23 @@
       <c r="AG18">
         <v>199</v>
       </c>
-    </row>
-    <row r="19" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH18">
+        <v>300</v>
+      </c>
+      <c r="AI18">
+        <v>150</v>
+      </c>
+      <c r="AJ18">
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>0</v>
+      </c>
+      <c r="AL18">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="19" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>51</v>
       </c>
@@ -2745,8 +3031,23 @@
       <c r="AG19">
         <v>199</v>
       </c>
-    </row>
-    <row r="20" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH19">
+        <v>100</v>
+      </c>
+      <c r="AI19">
+        <v>98</v>
+      </c>
+      <c r="AJ19">
+        <v>100</v>
+      </c>
+      <c r="AK19">
+        <v>0</v>
+      </c>
+      <c r="AL19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>52</v>
       </c>
@@ -2846,8 +3147,23 @@
       <c r="AG20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0</v>
+      </c>
+      <c r="AJ20">
+        <v>0</v>
+      </c>
+      <c r="AK20">
+        <v>0</v>
+      </c>
+      <c r="AL20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>53</v>
       </c>
@@ -2947,8 +3263,23 @@
       <c r="AG21">
         <v>300</v>
       </c>
-    </row>
-    <row r="22" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH21">
+        <v>300</v>
+      </c>
+      <c r="AI21">
+        <v>300</v>
+      </c>
+      <c r="AJ21">
+        <v>0</v>
+      </c>
+      <c r="AK21">
+        <v>0</v>
+      </c>
+      <c r="AL21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>54</v>
       </c>
@@ -3048,8 +3379,23 @@
       <c r="AG22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH22">
+        <v>200</v>
+      </c>
+      <c r="AI22">
+        <v>0</v>
+      </c>
+      <c r="AJ22">
+        <v>0</v>
+      </c>
+      <c r="AK22">
+        <v>0</v>
+      </c>
+      <c r="AL22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>55</v>
       </c>
@@ -3149,8 +3495,23 @@
       <c r="AG23">
         <v>2094</v>
       </c>
-    </row>
-    <row r="24" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH23">
+        <v>906</v>
+      </c>
+      <c r="AI23">
+        <v>1000</v>
+      </c>
+      <c r="AJ23">
+        <v>0</v>
+      </c>
+      <c r="AK23">
+        <v>1000</v>
+      </c>
+      <c r="AL23">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="24" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>56</v>
       </c>
@@ -3250,8 +3611,23 @@
       <c r="AG24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0</v>
+      </c>
+      <c r="AJ24">
+        <v>150</v>
+      </c>
+      <c r="AK24">
+        <v>0</v>
+      </c>
+      <c r="AL24">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="25" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>57</v>
       </c>
@@ -3351,8 +3727,23 @@
       <c r="AG25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH25">
+        <v>200</v>
+      </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>200</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="26" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>58</v>
       </c>
@@ -3452,8 +3843,23 @@
       <c r="AG26">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0</v>
+      </c>
+      <c r="AJ26">
+        <v>0</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>59</v>
       </c>
@@ -3553,8 +3959,23 @@
       <c r="AG27">
         <v>100</v>
       </c>
-    </row>
-    <row r="28" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH27">
+        <v>0</v>
+      </c>
+      <c r="AI27">
+        <v>0</v>
+      </c>
+      <c r="AJ27">
+        <v>100</v>
+      </c>
+      <c r="AK27">
+        <v>0</v>
+      </c>
+      <c r="AL27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>60</v>
       </c>
@@ -3654,8 +4075,23 @@
       <c r="AG28">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH28">
+        <v>0</v>
+      </c>
+      <c r="AI28">
+        <v>0</v>
+      </c>
+      <c r="AJ28">
+        <v>0</v>
+      </c>
+      <c r="AK28">
+        <v>0</v>
+      </c>
+      <c r="AL28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>61</v>
       </c>
@@ -3755,8 +4191,23 @@
       <c r="AG29">
         <v>0</v>
       </c>
-    </row>
-    <row r="30" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH29">
+        <v>300</v>
+      </c>
+      <c r="AI29">
+        <v>0</v>
+      </c>
+      <c r="AJ29">
+        <v>0</v>
+      </c>
+      <c r="AK29">
+        <v>300</v>
+      </c>
+      <c r="AL29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>62</v>
       </c>
@@ -3856,8 +4307,23 @@
       <c r="AG30">
         <v>0</v>
       </c>
-    </row>
-    <row r="31" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH30">
+        <v>0</v>
+      </c>
+      <c r="AI30">
+        <v>0</v>
+      </c>
+      <c r="AJ30">
+        <v>0</v>
+      </c>
+      <c r="AK30">
+        <v>0</v>
+      </c>
+      <c r="AL30">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="31" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>63</v>
       </c>
@@ -3957,8 +4423,23 @@
       <c r="AG31">
         <v>0</v>
       </c>
-    </row>
-    <row r="32" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH31">
+        <v>300</v>
+      </c>
+      <c r="AI31">
+        <v>0</v>
+      </c>
+      <c r="AJ31">
+        <v>0</v>
+      </c>
+      <c r="AK31">
+        <v>0</v>
+      </c>
+      <c r="AL31">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="32" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>64</v>
       </c>
@@ -4058,8 +4539,23 @@
       <c r="AG32">
         <v>0</v>
       </c>
-    </row>
-    <row r="33" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH32">
+        <v>300</v>
+      </c>
+      <c r="AI32">
+        <v>0</v>
+      </c>
+      <c r="AJ32">
+        <v>299</v>
+      </c>
+      <c r="AK32">
+        <v>0</v>
+      </c>
+      <c r="AL32">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="33" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>65</v>
       </c>
@@ -4159,8 +4655,23 @@
       <c r="AG33">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH33">
+        <v>0</v>
+      </c>
+      <c r="AI33">
+        <v>0</v>
+      </c>
+      <c r="AJ33">
+        <v>50</v>
+      </c>
+      <c r="AK33">
+        <v>0</v>
+      </c>
+      <c r="AL33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>66</v>
       </c>
@@ -4260,8 +4771,23 @@
       <c r="AG34">
         <v>0</v>
       </c>
-    </row>
-    <row r="35" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH34">
+        <v>0</v>
+      </c>
+      <c r="AI34">
+        <v>0</v>
+      </c>
+      <c r="AJ34">
+        <v>0</v>
+      </c>
+      <c r="AK34">
+        <v>0</v>
+      </c>
+      <c r="AL34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>67</v>
       </c>
@@ -4361,8 +4887,23 @@
       <c r="AG35">
         <v>100</v>
       </c>
-    </row>
-    <row r="36" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH35">
+        <v>0</v>
+      </c>
+      <c r="AI35">
+        <v>0</v>
+      </c>
+      <c r="AJ35">
+        <v>50</v>
+      </c>
+      <c r="AK35">
+        <v>0</v>
+      </c>
+      <c r="AL35">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -4462,8 +5003,23 @@
       <c r="AG36">
         <v>48</v>
       </c>
-    </row>
-    <row r="37" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH36">
+        <v>0</v>
+      </c>
+      <c r="AI36">
+        <v>50</v>
+      </c>
+      <c r="AJ36">
+        <v>48</v>
+      </c>
+      <c r="AK36">
+        <v>47</v>
+      </c>
+      <c r="AL36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -4563,8 +5119,23 @@
       <c r="AG37">
         <v>200</v>
       </c>
-    </row>
-    <row r="38" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH37">
+        <v>100</v>
+      </c>
+      <c r="AI37">
+        <v>177</v>
+      </c>
+      <c r="AJ37">
+        <v>76</v>
+      </c>
+      <c r="AK37">
+        <v>100</v>
+      </c>
+      <c r="AL37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>70</v>
       </c>
@@ -4664,8 +5235,23 @@
       <c r="AG38">
         <v>0</v>
       </c>
-    </row>
-    <row r="39" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH38">
+        <v>0</v>
+      </c>
+      <c r="AI38">
+        <v>0</v>
+      </c>
+      <c r="AJ38">
+        <v>99</v>
+      </c>
+      <c r="AK38">
+        <v>49</v>
+      </c>
+      <c r="AL38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>71</v>
       </c>
@@ -4765,8 +5351,23 @@
       <c r="AG39">
         <v>0</v>
       </c>
-    </row>
-    <row r="40" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH39">
+        <v>25</v>
+      </c>
+      <c r="AI39">
+        <v>25</v>
+      </c>
+      <c r="AJ39">
+        <v>30</v>
+      </c>
+      <c r="AK39">
+        <v>20</v>
+      </c>
+      <c r="AL39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>72</v>
       </c>
@@ -4866,8 +5467,23 @@
       <c r="AG40">
         <v>40</v>
       </c>
-    </row>
-    <row r="41" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH40">
+        <v>9</v>
+      </c>
+      <c r="AI40">
+        <v>0</v>
+      </c>
+      <c r="AJ40">
+        <v>0</v>
+      </c>
+      <c r="AK40">
+        <v>0</v>
+      </c>
+      <c r="AL40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>73</v>
       </c>
@@ -4967,8 +5583,23 @@
       <c r="AG41">
         <v>99</v>
       </c>
-    </row>
-    <row r="42" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH41">
+        <v>0</v>
+      </c>
+      <c r="AI41">
+        <v>49</v>
+      </c>
+      <c r="AJ41">
+        <v>50</v>
+      </c>
+      <c r="AK41">
+        <v>0</v>
+      </c>
+      <c r="AL41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>74</v>
       </c>
@@ -5068,8 +5699,23 @@
       <c r="AG42">
         <v>160</v>
       </c>
-    </row>
-    <row r="43" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH42">
+        <v>81</v>
+      </c>
+      <c r="AI42">
+        <v>116</v>
+      </c>
+      <c r="AJ42">
+        <v>105</v>
+      </c>
+      <c r="AK42">
+        <v>60</v>
+      </c>
+      <c r="AL42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>75</v>
       </c>
@@ -5169,8 +5815,23 @@
       <c r="AG43">
         <v>0</v>
       </c>
-    </row>
-    <row r="44" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH43">
+        <v>197</v>
+      </c>
+      <c r="AI43">
+        <v>299</v>
+      </c>
+      <c r="AJ43">
+        <v>0</v>
+      </c>
+      <c r="AK43">
+        <v>199</v>
+      </c>
+      <c r="AL43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>76</v>
       </c>
@@ -5270,8 +5931,23 @@
       <c r="AG44">
         <v>400</v>
       </c>
-    </row>
-    <row r="45" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH44">
+        <v>0</v>
+      </c>
+      <c r="AI44">
+        <v>400</v>
+      </c>
+      <c r="AJ44">
+        <v>100</v>
+      </c>
+      <c r="AK44">
+        <v>199</v>
+      </c>
+      <c r="AL44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>77</v>
       </c>
@@ -5371,8 +6047,23 @@
       <c r="AG45">
         <v>300</v>
       </c>
-    </row>
-    <row r="46" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH45">
+        <v>0</v>
+      </c>
+      <c r="AI45">
+        <v>800</v>
+      </c>
+      <c r="AJ45">
+        <v>0</v>
+      </c>
+      <c r="AK45">
+        <v>0</v>
+      </c>
+      <c r="AL45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>78</v>
       </c>
@@ -5472,8 +6163,23 @@
       <c r="AG46">
         <v>800</v>
       </c>
-    </row>
-    <row r="47" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH46">
+        <v>0</v>
+      </c>
+      <c r="AI46">
+        <v>500</v>
+      </c>
+      <c r="AJ46">
+        <v>500</v>
+      </c>
+      <c r="AK46">
+        <v>0</v>
+      </c>
+      <c r="AL46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>79</v>
       </c>
@@ -5573,8 +6279,23 @@
       <c r="AG47">
         <v>1499</v>
       </c>
-    </row>
-    <row r="48" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH47">
+        <v>1492</v>
+      </c>
+      <c r="AI47">
+        <v>2090</v>
+      </c>
+      <c r="AJ47">
+        <v>1993</v>
+      </c>
+      <c r="AK47">
+        <v>0</v>
+      </c>
+      <c r="AL47">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>80</v>
       </c>
@@ -5674,8 +6395,23 @@
       <c r="AG48">
         <v>134</v>
       </c>
-    </row>
-    <row r="49" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH48">
+        <v>161</v>
+      </c>
+      <c r="AI48">
+        <v>419</v>
+      </c>
+      <c r="AJ48">
+        <v>256</v>
+      </c>
+      <c r="AK48">
+        <v>331</v>
+      </c>
+      <c r="AL48">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="49" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>81</v>
       </c>
@@ -5775,8 +6511,23 @@
       <c r="AG49">
         <v>600</v>
       </c>
-    </row>
-    <row r="50" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH49">
+        <v>300</v>
+      </c>
+      <c r="AI49">
+        <v>200</v>
+      </c>
+      <c r="AJ49">
+        <v>0</v>
+      </c>
+      <c r="AK49">
+        <v>200</v>
+      </c>
+      <c r="AL49">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>82</v>
       </c>
@@ -5876,8 +6627,23 @@
       <c r="AG50">
         <v>99</v>
       </c>
-    </row>
-    <row r="51" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH50">
+        <v>0</v>
+      </c>
+      <c r="AI50">
+        <v>47</v>
+      </c>
+      <c r="AJ50">
+        <v>100</v>
+      </c>
+      <c r="AK50">
+        <v>0</v>
+      </c>
+      <c r="AL50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>83</v>
       </c>
@@ -5977,8 +6743,23 @@
       <c r="AG51">
         <v>498</v>
       </c>
-    </row>
-    <row r="52" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH51">
+        <v>300</v>
+      </c>
+      <c r="AI51">
+        <v>800</v>
+      </c>
+      <c r="AJ51">
+        <v>0</v>
+      </c>
+      <c r="AK51">
+        <v>600</v>
+      </c>
+      <c r="AL51">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>84</v>
       </c>
@@ -6078,8 +6859,23 @@
       <c r="AG52">
         <v>200</v>
       </c>
-    </row>
-    <row r="53" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH52">
+        <v>300</v>
+      </c>
+      <c r="AI52">
+        <v>400</v>
+      </c>
+      <c r="AJ52">
+        <v>100</v>
+      </c>
+      <c r="AK52">
+        <v>400</v>
+      </c>
+      <c r="AL52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>85</v>
       </c>
@@ -6179,8 +6975,23 @@
       <c r="AG53">
         <v>200</v>
       </c>
-    </row>
-    <row r="54" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH53">
+        <v>0</v>
+      </c>
+      <c r="AI53">
+        <v>0</v>
+      </c>
+      <c r="AJ53">
+        <v>200</v>
+      </c>
+      <c r="AK53">
+        <v>0</v>
+      </c>
+      <c r="AL53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -6280,8 +7091,23 @@
       <c r="AG54">
         <v>199</v>
       </c>
-    </row>
-    <row r="55" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH54">
+        <v>0</v>
+      </c>
+      <c r="AI54">
+        <v>29</v>
+      </c>
+      <c r="AJ54">
+        <v>100</v>
+      </c>
+      <c r="AK54">
+        <v>100</v>
+      </c>
+      <c r="AL54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>87</v>
       </c>
@@ -6381,8 +7207,23 @@
       <c r="AG55">
         <v>0</v>
       </c>
-    </row>
-    <row r="56" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH55">
+        <v>0</v>
+      </c>
+      <c r="AI55">
+        <v>0</v>
+      </c>
+      <c r="AJ55">
+        <v>0</v>
+      </c>
+      <c r="AK55">
+        <v>0</v>
+      </c>
+      <c r="AL55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>88</v>
       </c>
@@ -6482,8 +7323,23 @@
       <c r="AG56">
         <v>0</v>
       </c>
-    </row>
-    <row r="57" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH56">
+        <v>0</v>
+      </c>
+      <c r="AI56">
+        <v>0</v>
+      </c>
+      <c r="AJ56">
+        <v>0</v>
+      </c>
+      <c r="AK56">
+        <v>0</v>
+      </c>
+      <c r="AL56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>89</v>
       </c>
@@ -6583,8 +7439,23 @@
       <c r="AG57">
         <v>500</v>
       </c>
-    </row>
-    <row r="58" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH57">
+        <v>300</v>
+      </c>
+      <c r="AI57">
+        <v>377</v>
+      </c>
+      <c r="AJ57">
+        <v>190</v>
+      </c>
+      <c r="AK57">
+        <v>133</v>
+      </c>
+      <c r="AL57">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="58" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>90</v>
       </c>
@@ -6684,8 +7555,23 @@
       <c r="AG58">
         <v>300</v>
       </c>
-    </row>
-    <row r="59" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH58">
+        <v>100</v>
+      </c>
+      <c r="AI58">
+        <v>300</v>
+      </c>
+      <c r="AJ58">
+        <v>100</v>
+      </c>
+      <c r="AK58">
+        <v>100</v>
+      </c>
+      <c r="AL58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>91</v>
       </c>
@@ -6785,8 +7671,23 @@
       <c r="AG59">
         <v>200</v>
       </c>
-    </row>
-    <row r="60" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH59">
+        <v>0</v>
+      </c>
+      <c r="AI59">
+        <v>0</v>
+      </c>
+      <c r="AJ59">
+        <v>0</v>
+      </c>
+      <c r="AK59">
+        <v>0</v>
+      </c>
+      <c r="AL59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>92</v>
       </c>
@@ -6886,8 +7787,23 @@
       <c r="AG60">
         <v>90</v>
       </c>
-    </row>
-    <row r="61" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH60">
+        <v>98</v>
+      </c>
+      <c r="AI60">
+        <v>98</v>
+      </c>
+      <c r="AJ60">
+        <v>98</v>
+      </c>
+      <c r="AK60">
+        <v>92</v>
+      </c>
+      <c r="AL60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>93</v>
       </c>
@@ -6987,8 +7903,23 @@
       <c r="AG61">
         <v>0</v>
       </c>
-    </row>
-    <row r="62" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH61">
+        <v>99</v>
+      </c>
+      <c r="AI61">
+        <v>0</v>
+      </c>
+      <c r="AJ61">
+        <v>200</v>
+      </c>
+      <c r="AK61">
+        <v>98</v>
+      </c>
+      <c r="AL61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>94</v>
       </c>
@@ -7088,8 +8019,23 @@
       <c r="AG62">
         <v>595</v>
       </c>
-    </row>
-    <row r="63" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH62">
+        <v>600</v>
+      </c>
+      <c r="AI62">
+        <v>600</v>
+      </c>
+      <c r="AJ62">
+        <v>300</v>
+      </c>
+      <c r="AK62">
+        <v>300</v>
+      </c>
+      <c r="AL62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>95</v>
       </c>
@@ -7189,8 +8135,23 @@
       <c r="AG63">
         <v>200</v>
       </c>
-    </row>
-    <row r="64" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH63">
+        <v>99</v>
+      </c>
+      <c r="AI63">
+        <v>499</v>
+      </c>
+      <c r="AJ63">
+        <v>300</v>
+      </c>
+      <c r="AK63">
+        <v>0</v>
+      </c>
+      <c r="AL63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>96</v>
       </c>
@@ -7290,8 +8251,23 @@
       <c r="AG64">
         <v>200</v>
       </c>
-    </row>
-    <row r="65" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH64">
+        <v>600</v>
+      </c>
+      <c r="AI64">
+        <v>497</v>
+      </c>
+      <c r="AJ64">
+        <v>0</v>
+      </c>
+      <c r="AK64">
+        <v>250</v>
+      </c>
+      <c r="AL64">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="65" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>97</v>
       </c>
@@ -7391,8 +8367,23 @@
       <c r="AG65">
         <v>100</v>
       </c>
-    </row>
-    <row r="66" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH65">
+        <v>0</v>
+      </c>
+      <c r="AI65">
+        <v>0</v>
+      </c>
+      <c r="AJ65">
+        <v>99</v>
+      </c>
+      <c r="AK65">
+        <v>0</v>
+      </c>
+      <c r="AL65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>98</v>
       </c>
@@ -7492,8 +8483,23 @@
       <c r="AG66">
         <v>0</v>
       </c>
-    </row>
-    <row r="67" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH66">
+        <v>0</v>
+      </c>
+      <c r="AI66">
+        <v>0</v>
+      </c>
+      <c r="AJ66">
+        <v>0</v>
+      </c>
+      <c r="AK66">
+        <v>0</v>
+      </c>
+      <c r="AL66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>99</v>
       </c>
@@ -7593,8 +8599,23 @@
       <c r="AG67">
         <v>0</v>
       </c>
-    </row>
-    <row r="68" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH67">
+        <v>0</v>
+      </c>
+      <c r="AI67">
+        <v>0</v>
+      </c>
+      <c r="AJ67">
+        <v>0</v>
+      </c>
+      <c r="AK67">
+        <v>0</v>
+      </c>
+      <c r="AL67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>100</v>
       </c>
@@ -7694,8 +8715,23 @@
       <c r="AG68">
         <v>400</v>
       </c>
-    </row>
-    <row r="69" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH68">
+        <v>300</v>
+      </c>
+      <c r="AI68">
+        <v>500</v>
+      </c>
+      <c r="AJ68">
+        <v>250</v>
+      </c>
+      <c r="AK68">
+        <v>250</v>
+      </c>
+      <c r="AL68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>101</v>
       </c>
@@ -7795,8 +8831,23 @@
       <c r="AG69">
         <v>400</v>
       </c>
-    </row>
-    <row r="70" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH69">
+        <v>500</v>
+      </c>
+      <c r="AI69">
+        <v>500</v>
+      </c>
+      <c r="AJ69">
+        <v>500</v>
+      </c>
+      <c r="AK69">
+        <v>490</v>
+      </c>
+      <c r="AL69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>102</v>
       </c>
@@ -7896,8 +8947,23 @@
       <c r="AG70">
         <v>500</v>
       </c>
-    </row>
-    <row r="71" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH70">
+        <v>0</v>
+      </c>
+      <c r="AI70">
+        <v>500</v>
+      </c>
+      <c r="AJ70">
+        <v>300</v>
+      </c>
+      <c r="AK70">
+        <v>500</v>
+      </c>
+      <c r="AL70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>103</v>
       </c>
@@ -7997,8 +9063,23 @@
       <c r="AG71">
         <v>499</v>
       </c>
-    </row>
-    <row r="72" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH71">
+        <v>396</v>
+      </c>
+      <c r="AI71">
+        <v>395</v>
+      </c>
+      <c r="AJ71">
+        <v>494</v>
+      </c>
+      <c r="AK71">
+        <v>0</v>
+      </c>
+      <c r="AL71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>104</v>
       </c>
@@ -8098,8 +9179,23 @@
       <c r="AG72">
         <v>400</v>
       </c>
-    </row>
-    <row r="73" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH72">
+        <v>1000</v>
+      </c>
+      <c r="AI72">
+        <v>200</v>
+      </c>
+      <c r="AJ72">
+        <v>0</v>
+      </c>
+      <c r="AK72">
+        <v>797</v>
+      </c>
+      <c r="AL72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>105</v>
       </c>
@@ -8199,8 +9295,23 @@
       <c r="AG73">
         <v>496</v>
       </c>
-    </row>
-    <row r="74" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH73">
+        <v>0</v>
+      </c>
+      <c r="AI73">
+        <v>200</v>
+      </c>
+      <c r="AJ73">
+        <v>199</v>
+      </c>
+      <c r="AK73">
+        <v>0</v>
+      </c>
+      <c r="AL73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>106</v>
       </c>
@@ -8300,8 +9411,23 @@
       <c r="AG74">
         <v>699</v>
       </c>
-    </row>
-    <row r="75" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH74">
+        <v>0</v>
+      </c>
+      <c r="AI74">
+        <v>797</v>
+      </c>
+      <c r="AJ74">
+        <v>100</v>
+      </c>
+      <c r="AK74">
+        <v>44</v>
+      </c>
+      <c r="AL74">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="75" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>107</v>
       </c>
@@ -8401,8 +9527,23 @@
       <c r="AG75">
         <v>1492</v>
       </c>
-    </row>
-    <row r="76" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH75">
+        <v>1495</v>
+      </c>
+      <c r="AI75">
+        <v>300</v>
+      </c>
+      <c r="AJ75">
+        <v>1200</v>
+      </c>
+      <c r="AK75">
+        <v>591</v>
+      </c>
+      <c r="AL75">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="76" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>108</v>
       </c>
@@ -8502,8 +9643,23 @@
       <c r="AG76">
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH76">
+        <v>0</v>
+      </c>
+      <c r="AI76">
+        <v>0</v>
+      </c>
+      <c r="AJ76">
+        <v>0</v>
+      </c>
+      <c r="AK76">
+        <v>0</v>
+      </c>
+      <c r="AL76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>109</v>
       </c>
@@ -8603,8 +9759,23 @@
       <c r="AG77">
         <v>160</v>
       </c>
-    </row>
-    <row r="78" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH77">
+        <v>100</v>
+      </c>
+      <c r="AI77">
+        <v>100</v>
+      </c>
+      <c r="AJ77">
+        <v>101</v>
+      </c>
+      <c r="AK77">
+        <v>100</v>
+      </c>
+      <c r="AL77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>110</v>
       </c>
@@ -8704,8 +9875,23 @@
       <c r="AG78">
         <v>490</v>
       </c>
-    </row>
-    <row r="79" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH78">
+        <v>0</v>
+      </c>
+      <c r="AI78">
+        <v>300</v>
+      </c>
+      <c r="AJ78">
+        <v>0</v>
+      </c>
+      <c r="AK78">
+        <v>0</v>
+      </c>
+      <c r="AL78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>111</v>
       </c>
@@ -8805,8 +9991,23 @@
       <c r="AG79">
         <v>1603</v>
       </c>
-    </row>
-    <row r="80" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH79">
+        <v>1001</v>
+      </c>
+      <c r="AI79">
+        <v>800</v>
+      </c>
+      <c r="AJ79">
+        <v>402</v>
+      </c>
+      <c r="AK79">
+        <v>0</v>
+      </c>
+      <c r="AL79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>112</v>
       </c>
@@ -8906,8 +10107,23 @@
       <c r="AG80">
         <v>0</v>
       </c>
-    </row>
-    <row r="81" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH80">
+        <v>0</v>
+      </c>
+      <c r="AI80">
+        <v>0</v>
+      </c>
+      <c r="AJ80">
+        <v>0</v>
+      </c>
+      <c r="AK80">
+        <v>0</v>
+      </c>
+      <c r="AL80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>113</v>
       </c>
@@ -9007,8 +10223,23 @@
       <c r="AG81">
         <v>700</v>
       </c>
-    </row>
-    <row r="82" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH81">
+        <v>498</v>
+      </c>
+      <c r="AI81">
+        <v>497</v>
+      </c>
+      <c r="AJ81">
+        <v>996</v>
+      </c>
+      <c r="AK81">
+        <v>0</v>
+      </c>
+      <c r="AL81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>114</v>
       </c>
@@ -9108,8 +10339,23 @@
       <c r="AG82">
         <v>100</v>
       </c>
-    </row>
-    <row r="83" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH82">
+        <v>0</v>
+      </c>
+      <c r="AI82">
+        <v>0</v>
+      </c>
+      <c r="AJ82">
+        <v>200</v>
+      </c>
+      <c r="AK82">
+        <v>0</v>
+      </c>
+      <c r="AL82">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="83" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>115</v>
       </c>
@@ -9209,8 +10455,23 @@
       <c r="AG83">
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH83">
+        <v>0</v>
+      </c>
+      <c r="AI83">
+        <v>0</v>
+      </c>
+      <c r="AJ83">
+        <v>0</v>
+      </c>
+      <c r="AK83">
+        <v>0</v>
+      </c>
+      <c r="AL83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>116</v>
       </c>
@@ -9310,8 +10571,23 @@
       <c r="AG84">
         <v>700</v>
       </c>
-    </row>
-    <row r="85" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH84">
+        <v>700</v>
+      </c>
+      <c r="AI84">
+        <v>500</v>
+      </c>
+      <c r="AJ84">
+        <v>500</v>
+      </c>
+      <c r="AK84">
+        <v>0</v>
+      </c>
+      <c r="AL84">
+        <v>499</v>
+      </c>
+    </row>
+    <row r="85" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>117</v>
       </c>
@@ -9411,8 +10687,23 @@
       <c r="AG85">
         <v>500</v>
       </c>
-    </row>
-    <row r="86" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH85">
+        <v>600</v>
+      </c>
+      <c r="AI85">
+        <v>500</v>
+      </c>
+      <c r="AJ85">
+        <v>500</v>
+      </c>
+      <c r="AK85">
+        <v>282</v>
+      </c>
+      <c r="AL85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>118</v>
       </c>
@@ -9512,8 +10803,23 @@
       <c r="AG86">
         <v>99</v>
       </c>
-    </row>
-    <row r="87" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH86">
+        <v>99</v>
+      </c>
+      <c r="AI86">
+        <v>99</v>
+      </c>
+      <c r="AJ86">
+        <v>101</v>
+      </c>
+      <c r="AK86">
+        <v>99</v>
+      </c>
+      <c r="AL86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>119</v>
       </c>
@@ -9613,8 +10919,23 @@
       <c r="AG87">
         <v>800</v>
       </c>
-    </row>
-    <row r="88" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH87">
+        <v>1300</v>
+      </c>
+      <c r="AI87">
+        <v>700</v>
+      </c>
+      <c r="AJ87">
+        <v>998</v>
+      </c>
+      <c r="AK87">
+        <v>0</v>
+      </c>
+      <c r="AL87">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="88" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>120</v>
       </c>
@@ -9714,8 +11035,23 @@
       <c r="AG88">
         <v>490</v>
       </c>
-    </row>
-    <row r="89" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH88">
+        <v>690</v>
+      </c>
+      <c r="AI88">
+        <v>490</v>
+      </c>
+      <c r="AJ88">
+        <v>0</v>
+      </c>
+      <c r="AK88">
+        <v>95</v>
+      </c>
+      <c r="AL88">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="89" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>121</v>
       </c>
@@ -9815,8 +11151,23 @@
       <c r="AG89">
         <v>500</v>
       </c>
-    </row>
-    <row r="90" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH89">
+        <v>499.99968181818178</v>
+      </c>
+      <c r="AI89">
+        <v>500</v>
+      </c>
+      <c r="AJ89">
+        <v>300</v>
+      </c>
+      <c r="AK89">
+        <v>0</v>
+      </c>
+      <c r="AL89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>122</v>
       </c>
@@ -9916,8 +11267,23 @@
       <c r="AG90">
         <v>495</v>
       </c>
-    </row>
-    <row r="91" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH90">
+        <v>498</v>
+      </c>
+      <c r="AI90">
+        <v>499</v>
+      </c>
+      <c r="AJ90">
+        <v>0</v>
+      </c>
+      <c r="AK90">
+        <v>0</v>
+      </c>
+      <c r="AL90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>123</v>
       </c>
@@ -10017,8 +11383,23 @@
       <c r="AG91">
         <v>300</v>
       </c>
-    </row>
-    <row r="92" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH91">
+        <v>400</v>
+      </c>
+      <c r="AI91">
+        <v>300</v>
+      </c>
+      <c r="AJ91">
+        <v>300</v>
+      </c>
+      <c r="AK91">
+        <v>0</v>
+      </c>
+      <c r="AL91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>124</v>
       </c>
@@ -10118,8 +11499,23 @@
       <c r="AG92">
         <v>200</v>
       </c>
-    </row>
-    <row r="93" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH92">
+        <v>300</v>
+      </c>
+      <c r="AI92">
+        <v>0</v>
+      </c>
+      <c r="AJ92">
+        <v>0</v>
+      </c>
+      <c r="AK92">
+        <v>0</v>
+      </c>
+      <c r="AL92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>125</v>
       </c>
@@ -10219,8 +11615,23 @@
       <c r="AG93">
         <v>0</v>
       </c>
-    </row>
-    <row r="94" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH93">
+        <v>0</v>
+      </c>
+      <c r="AI93">
+        <v>0</v>
+      </c>
+      <c r="AJ93">
+        <v>0</v>
+      </c>
+      <c r="AK93">
+        <v>0</v>
+      </c>
+      <c r="AL93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>126</v>
       </c>
@@ -10320,8 +11731,23 @@
       <c r="AG94">
         <v>2000</v>
       </c>
-    </row>
-    <row r="95" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH94">
+        <v>1000</v>
+      </c>
+      <c r="AI94">
+        <v>0</v>
+      </c>
+      <c r="AJ94">
+        <v>1200</v>
+      </c>
+      <c r="AK94">
+        <v>0</v>
+      </c>
+      <c r="AL94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>127</v>
       </c>
@@ -10421,8 +11847,23 @@
       <c r="AG95">
         <v>1000</v>
       </c>
-    </row>
-    <row r="96" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH95">
+        <v>1001</v>
+      </c>
+      <c r="AI95">
+        <v>0</v>
+      </c>
+      <c r="AJ95">
+        <v>1000</v>
+      </c>
+      <c r="AK95">
+        <v>0</v>
+      </c>
+      <c r="AL95">
+        <v>2600</v>
+      </c>
+    </row>
+    <row r="96" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>128</v>
       </c>
@@ -10522,8 +11963,23 @@
       <c r="AG96">
         <v>199</v>
       </c>
-    </row>
-    <row r="97" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH96">
+        <v>697</v>
+      </c>
+      <c r="AI96">
+        <v>199</v>
+      </c>
+      <c r="AJ96">
+        <v>299</v>
+      </c>
+      <c r="AK96">
+        <v>0</v>
+      </c>
+      <c r="AL96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>129</v>
       </c>
@@ -10623,8 +12079,23 @@
       <c r="AG97">
         <v>1000</v>
       </c>
-    </row>
-    <row r="98" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH97">
+        <v>999</v>
+      </c>
+      <c r="AI97">
+        <v>1001</v>
+      </c>
+      <c r="AJ97">
+        <v>499</v>
+      </c>
+      <c r="AK97">
+        <v>0</v>
+      </c>
+      <c r="AL97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>130</v>
       </c>
@@ -10724,8 +12195,23 @@
       <c r="AG98">
         <v>650</v>
       </c>
-    </row>
-    <row r="99" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH98">
+        <v>0</v>
+      </c>
+      <c r="AI98">
+        <v>0</v>
+      </c>
+      <c r="AJ98">
+        <v>300</v>
+      </c>
+      <c r="AK98">
+        <v>0</v>
+      </c>
+      <c r="AL98">
+        <v>1300</v>
+      </c>
+    </row>
+    <row r="99" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>131</v>
       </c>
@@ -10825,8 +12311,23 @@
       <c r="AG99">
         <v>0</v>
       </c>
-    </row>
-    <row r="100" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH99">
+        <v>200</v>
+      </c>
+      <c r="AI99">
+        <v>200</v>
+      </c>
+      <c r="AJ99">
+        <v>0</v>
+      </c>
+      <c r="AK99">
+        <v>50</v>
+      </c>
+      <c r="AL99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>132</v>
       </c>
@@ -10926,8 +12427,23 @@
       <c r="AG100">
         <v>300</v>
       </c>
-    </row>
-    <row r="101" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH100">
+        <v>300</v>
+      </c>
+      <c r="AI100">
+        <v>300</v>
+      </c>
+      <c r="AJ100">
+        <v>198</v>
+      </c>
+      <c r="AK100">
+        <v>0</v>
+      </c>
+      <c r="AL100">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="101" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>133</v>
       </c>
@@ -11027,8 +12543,23 @@
       <c r="AG101">
         <v>298</v>
       </c>
-    </row>
-    <row r="102" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH101">
+        <v>198</v>
+      </c>
+      <c r="AI101">
+        <v>0</v>
+      </c>
+      <c r="AJ101">
+        <v>0</v>
+      </c>
+      <c r="AK101">
+        <v>0</v>
+      </c>
+      <c r="AL101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>134</v>
       </c>
@@ -11128,8 +12659,23 @@
       <c r="AG102">
         <v>500</v>
       </c>
-    </row>
-    <row r="103" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH102">
+        <v>0</v>
+      </c>
+      <c r="AI102">
+        <v>795</v>
+      </c>
+      <c r="AJ102">
+        <v>500</v>
+      </c>
+      <c r="AK102">
+        <v>500</v>
+      </c>
+      <c r="AL102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>135</v>
       </c>
@@ -11229,8 +12775,23 @@
       <c r="AG103">
         <v>700</v>
       </c>
-    </row>
-    <row r="104" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH103">
+        <v>1400</v>
+      </c>
+      <c r="AI103">
+        <v>500</v>
+      </c>
+      <c r="AJ103">
+        <v>310</v>
+      </c>
+      <c r="AK103">
+        <v>0</v>
+      </c>
+      <c r="AL103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>136</v>
       </c>
@@ -11330,8 +12891,23 @@
       <c r="AG104">
         <v>300</v>
       </c>
-    </row>
-    <row r="105" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH104">
+        <v>300</v>
+      </c>
+      <c r="AI104">
+        <v>0</v>
+      </c>
+      <c r="AJ104">
+        <v>300</v>
+      </c>
+      <c r="AK104">
+        <v>286</v>
+      </c>
+      <c r="AL104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>137</v>
       </c>
@@ -11431,8 +13007,23 @@
       <c r="AG105">
         <v>1000</v>
       </c>
-    </row>
-    <row r="106" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH105">
+        <v>1000</v>
+      </c>
+      <c r="AI105">
+        <v>1000</v>
+      </c>
+      <c r="AJ105">
+        <v>0</v>
+      </c>
+      <c r="AK105">
+        <v>0</v>
+      </c>
+      <c r="AL105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>138</v>
       </c>
@@ -11532,8 +13123,23 @@
       <c r="AG106">
         <v>300</v>
       </c>
-    </row>
-    <row r="107" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH106">
+        <v>300</v>
+      </c>
+      <c r="AI106">
+        <v>199</v>
+      </c>
+      <c r="AJ106">
+        <v>0</v>
+      </c>
+      <c r="AK106">
+        <v>199</v>
+      </c>
+      <c r="AL106">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="107" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>139</v>
       </c>
@@ -11633,8 +13239,23 @@
       <c r="AG107">
         <v>700</v>
       </c>
-    </row>
-    <row r="108" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH107">
+        <v>500</v>
+      </c>
+      <c r="AI107">
+        <v>200</v>
+      </c>
+      <c r="AJ107">
+        <v>100</v>
+      </c>
+      <c r="AK107">
+        <v>0</v>
+      </c>
+      <c r="AL107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>140</v>
       </c>
@@ -11734,8 +13355,23 @@
       <c r="AG108">
         <v>400</v>
       </c>
-    </row>
-    <row r="109" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH108">
+        <v>791</v>
+      </c>
+      <c r="AI108">
+        <v>0</v>
+      </c>
+      <c r="AJ108">
+        <v>290</v>
+      </c>
+      <c r="AK108">
+        <v>387</v>
+      </c>
+      <c r="AL108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>141</v>
       </c>
@@ -11835,8 +13471,23 @@
       <c r="AG109">
         <v>400</v>
       </c>
-    </row>
-    <row r="110" spans="1:33" x14ac:dyDescent="0.3">
+      <c r="AH109">
+        <v>100</v>
+      </c>
+      <c r="AI109">
+        <v>200</v>
+      </c>
+      <c r="AJ109">
+        <v>200</v>
+      </c>
+      <c r="AK109">
+        <v>98</v>
+      </c>
+      <c r="AL109">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="110" spans="1:38" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>142</v>
       </c>
@@ -11936,9 +13587,25 @@
       <c r="AG110">
         <v>399</v>
       </c>
+      <c r="AH110">
+        <v>700</v>
+      </c>
+      <c r="AI110">
+        <v>698</v>
+      </c>
+      <c r="AJ110">
+        <v>998</v>
+      </c>
+      <c r="AK110">
+        <v>0</v>
+      </c>
+      <c r="AL110">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -11946,8 +13613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F029559-D218-485C-A850-ABE2CD583F18}">
   <dimension ref="A1:B110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A101" workbookViewId="0">
-      <selection activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11977,7 +13644,7 @@
         <v>35</v>
       </c>
       <c r="B3">
-        <v>3276</v>
+        <v>3576</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -11985,7 +13652,7 @@
         <v>36</v>
       </c>
       <c r="B4">
-        <v>4907</v>
+        <v>5627</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -12001,7 +13668,7 @@
         <v>38</v>
       </c>
       <c r="B6">
-        <v>3765</v>
+        <v>5463</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -12009,7 +13676,7 @@
         <v>39</v>
       </c>
       <c r="B7">
-        <v>12379</v>
+        <v>12997</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -12017,7 +13684,7 @@
         <v>40</v>
       </c>
       <c r="B8">
-        <v>553</v>
+        <v>728</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -12025,7 +13692,7 @@
         <v>41</v>
       </c>
       <c r="B9">
-        <v>4270</v>
+        <v>4674</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -12033,7 +13700,7 @@
         <v>42</v>
       </c>
       <c r="B10">
-        <v>4550</v>
+        <v>4890</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -12041,7 +13708,7 @@
         <v>43</v>
       </c>
       <c r="B11">
-        <v>15519</v>
+        <v>16864</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -12049,7 +13716,7 @@
         <v>44</v>
       </c>
       <c r="B12">
-        <v>4915</v>
+        <v>5860</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -12057,7 +13724,7 @@
         <v>45</v>
       </c>
       <c r="B13">
-        <v>7834</v>
+        <v>9889</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -12065,7 +13732,7 @@
         <v>46</v>
       </c>
       <c r="B14">
-        <v>5687</v>
+        <v>6492</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -12073,7 +13740,7 @@
         <v>47</v>
       </c>
       <c r="B15">
-        <v>12530</v>
+        <v>14857</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -12081,7 +13748,7 @@
         <v>48</v>
       </c>
       <c r="B16">
-        <v>7551</v>
+        <v>8770</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -12089,7 +13756,7 @@
         <v>49</v>
       </c>
       <c r="B17">
-        <v>11150</v>
+        <v>11805</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -12097,7 +13764,7 @@
         <v>50</v>
       </c>
       <c r="B18">
-        <v>6561</v>
+        <v>7080</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -12105,7 +13772,7 @@
         <v>51</v>
       </c>
       <c r="B19">
-        <v>3042</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -12121,7 +13788,7 @@
         <v>53</v>
       </c>
       <c r="B21">
-        <v>15307</v>
+        <v>16084</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -12129,7 +13796,7 @@
         <v>54</v>
       </c>
       <c r="B22">
-        <v>4760</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -12137,7 +13804,7 @@
         <v>55</v>
       </c>
       <c r="B23">
-        <v>13546</v>
+        <v>18435</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -12145,7 +13812,7 @@
         <v>56</v>
       </c>
       <c r="B24">
-        <v>11345</v>
+        <v>11650</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -12153,7 +13820,7 @@
         <v>57</v>
       </c>
       <c r="B25">
-        <v>7508</v>
+        <v>8007</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -12161,7 +13828,7 @@
         <v>58</v>
       </c>
       <c r="B26">
-        <v>14527</v>
+        <v>14606</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -12169,7 +13836,7 @@
         <v>59</v>
       </c>
       <c r="B27">
-        <v>3929</v>
+        <v>4129</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -12185,7 +13852,7 @@
         <v>61</v>
       </c>
       <c r="B29">
-        <v>6280</v>
+        <v>6752</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -12193,7 +13860,7 @@
         <v>62</v>
       </c>
       <c r="B30">
-        <v>1685</v>
+        <v>1800</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -12201,7 +13868,7 @@
         <v>63</v>
       </c>
       <c r="B31">
-        <v>7928</v>
+        <v>8137</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -12209,7 +13876,7 @@
         <v>64</v>
       </c>
       <c r="B32">
-        <v>7405</v>
+        <v>8169</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -12217,7 +13884,7 @@
         <v>65</v>
       </c>
       <c r="B33">
-        <v>2543</v>
+        <v>2630</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -12225,7 +13892,7 @@
         <v>66</v>
       </c>
       <c r="B34">
-        <v>2222</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -12233,7 +13900,7 @@
         <v>67</v>
       </c>
       <c r="B35">
-        <v>2769</v>
+        <v>2891</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -12241,7 +13908,7 @@
         <v>68</v>
       </c>
       <c r="B36">
-        <v>1915</v>
+        <v>2078</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -12249,7 +13916,7 @@
         <v>69</v>
       </c>
       <c r="B37">
-        <v>7920</v>
+        <v>8600</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -12257,7 +13924,7 @@
         <v>70</v>
       </c>
       <c r="B38">
-        <v>2183</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -12265,7 +13932,7 @@
         <v>71</v>
       </c>
       <c r="B39">
-        <v>2030</v>
+        <v>2095</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -12273,7 +13940,7 @@
         <v>72</v>
       </c>
       <c r="B40">
-        <v>1385</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -12281,7 +13948,7 @@
         <v>73</v>
       </c>
       <c r="B41">
-        <v>2204</v>
+        <v>2384</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -12289,7 +13956,7 @@
         <v>74</v>
       </c>
       <c r="B42">
-        <v>9751</v>
+        <v>10570</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -12297,7 +13964,7 @@
         <v>75</v>
       </c>
       <c r="B43">
-        <v>10567</v>
+        <v>11300</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -12305,7 +13972,7 @@
         <v>76</v>
       </c>
       <c r="B44">
-        <v>9122</v>
+        <v>10317</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -12313,7 +13980,7 @@
         <v>77</v>
       </c>
       <c r="B45">
-        <v>9550</v>
+        <v>10590</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -12321,7 +13988,7 @@
         <v>78</v>
       </c>
       <c r="B46">
-        <v>11200</v>
+        <v>12775</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -12329,7 +13996,7 @@
         <v>79</v>
       </c>
       <c r="B47">
-        <v>13594</v>
+        <v>20148</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -12337,7 +14004,7 @@
         <v>80</v>
       </c>
       <c r="B48">
-        <v>8997</v>
+        <v>10017</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -12345,7 +14012,7 @@
         <v>81</v>
       </c>
       <c r="B49">
-        <v>6962</v>
+        <v>8236</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -12353,7 +14020,7 @@
         <v>82</v>
       </c>
       <c r="B50">
-        <v>3511</v>
+        <v>3746</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -12361,7 +14028,7 @@
         <v>83</v>
       </c>
       <c r="B51">
-        <v>11271</v>
+        <v>13575</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -12369,7 +14036,7 @@
         <v>84</v>
       </c>
       <c r="B52">
-        <v>8320</v>
+        <v>9590</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -12377,7 +14044,7 @@
         <v>85</v>
       </c>
       <c r="B53">
-        <v>7160</v>
+        <v>7518</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -12385,7 +14052,7 @@
         <v>86</v>
       </c>
       <c r="B54">
-        <v>7278</v>
+        <v>7725</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -12393,7 +14060,7 @@
         <v>87</v>
       </c>
       <c r="B55">
-        <v>4450</v>
+        <v>4490</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -12401,7 +14068,7 @@
         <v>88</v>
       </c>
       <c r="B56">
-        <v>1118</v>
+        <v>1168</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -12409,7 +14076,7 @@
         <v>89</v>
       </c>
       <c r="B57">
-        <v>12320</v>
+        <v>13800</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -12417,7 +14084,7 @@
         <v>90</v>
       </c>
       <c r="B58">
-        <v>6241</v>
+        <v>7225</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -12425,7 +14092,7 @@
         <v>91</v>
       </c>
       <c r="B59">
-        <v>35800</v>
+        <v>36250</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -12433,7 +14100,7 @@
         <v>92</v>
       </c>
       <c r="B60">
-        <v>4050</v>
+        <v>4350</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -12441,7 +14108,7 @@
         <v>93</v>
       </c>
       <c r="B61">
-        <v>6263</v>
+        <v>6613</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -12449,7 +14116,7 @@
         <v>94</v>
       </c>
       <c r="B62">
-        <v>34490</v>
+        <v>36640</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -12457,7 +14124,7 @@
         <v>95</v>
       </c>
       <c r="B63">
-        <v>11466</v>
+        <v>12310</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -12465,7 +14132,7 @@
         <v>96</v>
       </c>
       <c r="B64">
-        <v>9931</v>
+        <v>11530</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -12473,7 +14140,7 @@
         <v>97</v>
       </c>
       <c r="B65">
-        <v>5366</v>
+        <v>5581</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -12489,7 +14156,7 @@
         <v>99</v>
       </c>
       <c r="B67">
-        <v>33660</v>
+        <v>33950</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -12497,7 +14164,7 @@
         <v>100</v>
       </c>
       <c r="B68">
-        <v>9415</v>
+        <v>11129</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -12505,7 +14172,7 @@
         <v>101</v>
       </c>
       <c r="B69">
-        <v>37650</v>
+        <v>39253</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -12513,7 +14180,7 @@
         <v>102</v>
       </c>
       <c r="B70">
-        <v>36488</v>
+        <v>38365</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -12521,7 +14188,7 @@
         <v>103</v>
       </c>
       <c r="B71">
-        <v>17095</v>
+        <v>18625</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -12529,7 +14196,7 @@
         <v>104</v>
       </c>
       <c r="B72">
-        <v>25650</v>
+        <v>28050</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -12537,7 +14204,7 @@
         <v>105</v>
       </c>
       <c r="B73">
-        <v>9476</v>
+        <v>10350</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -12545,7 +14212,7 @@
         <v>106</v>
       </c>
       <c r="B74">
-        <v>17000</v>
+        <v>19000</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -12553,7 +14220,7 @@
         <v>107</v>
       </c>
       <c r="B75">
-        <v>27047</v>
+        <v>32082</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -12569,7 +14236,7 @@
         <v>109</v>
       </c>
       <c r="B77">
-        <v>5290</v>
+        <v>5691</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -12577,7 +14244,7 @@
         <v>110</v>
       </c>
       <c r="B78">
-        <v>21986</v>
+        <v>22976</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -12585,7 +14252,7 @@
         <v>111</v>
       </c>
       <c r="B79">
-        <v>18455</v>
+        <v>21655</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -12601,7 +14268,7 @@
         <v>113</v>
       </c>
       <c r="B81">
-        <v>21020</v>
+        <v>23270</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -12609,7 +14276,7 @@
         <v>114</v>
       </c>
       <c r="B82">
-        <v>6459</v>
+        <v>6880</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -12625,7 +14292,7 @@
         <v>116</v>
       </c>
       <c r="B84">
-        <v>20333</v>
+        <v>23688</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -12633,7 +14300,7 @@
         <v>117</v>
       </c>
       <c r="B85">
-        <v>20300</v>
+        <v>22450</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -12641,7 +14308,7 @@
         <v>118</v>
       </c>
       <c r="B86">
-        <v>12543</v>
+        <v>13050</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -12649,7 +14316,7 @@
         <v>119</v>
       </c>
       <c r="B87">
-        <v>22190</v>
+        <v>27170</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -12657,7 +14324,7 @@
         <v>120</v>
       </c>
       <c r="B88">
-        <v>13716</v>
+        <v>15626</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -12665,7 +14332,7 @@
         <v>121</v>
       </c>
       <c r="B89">
-        <v>27437</v>
+        <v>29050</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -12673,7 +14340,7 @@
         <v>122</v>
       </c>
       <c r="B90">
-        <v>14505</v>
+        <v>15873</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -12681,7 +14348,7 @@
         <v>123</v>
       </c>
       <c r="B91">
-        <v>16360</v>
+        <v>17564</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -12689,7 +14356,7 @@
         <v>124</v>
       </c>
       <c r="B92">
-        <v>4200</v>
+        <v>4783</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -12705,7 +14372,7 @@
         <v>126</v>
       </c>
       <c r="B94">
-        <v>29939</v>
+        <v>33241</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -12713,7 +14380,7 @@
         <v>127</v>
       </c>
       <c r="B95">
-        <v>14888</v>
+        <v>19969</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -12721,7 +14388,7 @@
         <v>128</v>
       </c>
       <c r="B96">
-        <v>17016</v>
+        <v>18796</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -12729,7 +14396,7 @@
         <v>129</v>
       </c>
       <c r="B97">
-        <v>21600</v>
+        <v>24850</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -12737,7 +14404,7 @@
         <v>130</v>
       </c>
       <c r="B98">
-        <v>9182</v>
+        <v>11100</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -12745,7 +14412,7 @@
         <v>131</v>
       </c>
       <c r="B99">
-        <v>2664</v>
+        <v>2920</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -12753,7 +14420,7 @@
         <v>132</v>
       </c>
       <c r="B100">
-        <v>9250</v>
+        <v>10500</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -12761,7 +14428,7 @@
         <v>133</v>
       </c>
       <c r="B101">
-        <v>4638</v>
+        <v>5036</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -12769,7 +14436,7 @@
         <v>134</v>
       </c>
       <c r="B102">
-        <v>7515</v>
+        <v>9876</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -12777,7 +14444,7 @@
         <v>135</v>
       </c>
       <c r="B103">
-        <v>14250</v>
+        <v>16750</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -12785,7 +14452,7 @@
         <v>136</v>
       </c>
       <c r="B104">
-        <v>22563</v>
+        <v>23500</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -12793,7 +14460,7 @@
         <v>137</v>
       </c>
       <c r="B105">
-        <v>23502</v>
+        <v>26193</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -12801,7 +14468,7 @@
         <v>138</v>
       </c>
       <c r="B106">
-        <v>9330</v>
+        <v>10248</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -12809,7 +14476,7 @@
         <v>139</v>
       </c>
       <c r="B107">
-        <v>18360</v>
+        <v>19480</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -12817,7 +14484,7 @@
         <v>140</v>
       </c>
       <c r="B108">
-        <v>27342</v>
+        <v>28875</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -12825,7 +14492,7 @@
         <v>141</v>
       </c>
       <c r="B109">
-        <v>8621</v>
+        <v>9523</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -12833,7 +14500,7 @@
         <v>142</v>
       </c>
       <c r="B110">
-        <v>18956</v>
+        <v>20881</v>
       </c>
     </row>
   </sheetData>

</xml_diff>